<commit_message>
Thêm tính năng đọc dữ liệu từ file và ghi truyền vào login
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam 4\ThucTap\SystemTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78BA6588-1297-42B1-B9C1-DA78DEA5909C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1340A2EC-A5ED-44B0-B22A-65CCE9963815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F505DD84-6525-4D5C-B30B-B9CE41BF9A9D}"/>
+    <workbookView xWindow="3825" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{F505DD84-6525-4D5C-B30B-B9CE41BF9A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,13 +414,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Thêm tính năng random time và một vài thứ nho nhỏ
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam 4\ThucTap\SystemTest\src\test\resources\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -49,12 +49,16 @@
   </si>
   <si>
     <t>nhanviendien</t>
+  </si>
+  <si>
+    <t>New Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,8 +423,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>